<commit_message>
Record sales and returns
</commit_message>
<xml_diff>
--- a/sales_records.xlsx
+++ b/sales_records.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,51 +466,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>INV000001</t>
+          <t>INV000002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:08</t>
+          <t>2024-06-29 10:32:21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>E24062900001</t>
+          <t>J24062900002</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>παντελονι</t>
+          <t>ζωνη</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INV000001</t>
+          <t>INV000002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:08</t>
+          <t>2024-06-29 10:32:21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E24062900002</t>
+          <t>I24062900001</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>παντελονι</t>
+          <t>μπουφαν</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -526,132 +526,132 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>J24062900001</t>
+          <t>I24062900002</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ζωνη</t>
+          <t>μπουφαν</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INV000002</t>
+          <t>INV000003</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:21</t>
+          <t>2024-06-29 10:32:50</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>J24062900002</t>
+          <t>A24062900002</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ζωνη</t>
+          <t>φορεμα</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INV000002</t>
+          <t>INV000004</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:21</t>
+          <t>2024-06-29 19:27:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>I24062900001</t>
+          <t>A24062900004</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>μπουφαν</t>
+          <t>φορεμα</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INV000002</t>
+          <t>INV000005</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:21</t>
+          <t>2024-06-30 10:45:56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>I24062900002</t>
+          <t>A24063000002</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>μπουφαν</t>
+          <t>φορεμα</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>INV000003</t>
+          <t>INV000006</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:50</t>
+          <t>2024-06-30 10:46:52</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A24062900001</t>
+          <t>J24063000001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>φορεμα</t>
+          <t>ζωνη</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INV000003</t>
+          <t>INV000007</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-06-29 10:32:50</t>
+          <t>2024-07-03 19:44:21</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A24062900002</t>
+          <t>A24070300001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -660,7 +660,807 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>INV000008</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:46:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>J24070300001</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>INV000008</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:46:11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>J24070300002</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>INV000009</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:47:20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>H24070300001</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>πουκαμισο</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>INV000009</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:47:20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>H24070300002</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>πουκαμισο</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>INV000010</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:51:08</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>I24070300001</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>INV000010</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:51:08</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>I24070300002</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>INV000010</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:51:08</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>I24070300003</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>INV000011</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:52:47</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>I24070300004</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>INV000011</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:52:47</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>I24070300005</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>INV000011</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:52:47</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>I24070300006</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>INV000011</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:52:47</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>B24070300001</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>φανελα</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>INV000011</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:52:47</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>B24070300002</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>φανελα</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>I24070300007</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>I24070300008</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>I24070300009</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>B24070300003</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>φανελα</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>B24070300004</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>φανελα</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>INV000012</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:55:12</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>D24070300001</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>σορτσακι</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>INV000013</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:58:53</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>J24070300003</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>INV000013</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:58:53</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>J24070300004</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>INV000013</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:58:53</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>I24070300010</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>INV000013</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:58:53</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>I24070300011</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>INV000013</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2024-07-03 19:58:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>I24070300012</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>INV000014</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:00:41</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>I24070300013</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>INV000014</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:00:41</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>I24070300014</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>INV000014</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:00:41</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>J24070300005</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>INV000015</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:01:43</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>I24070300015</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>INV000015</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:01:43</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>I24070300016</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>μπουφαν</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>INV000016</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:02:49</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>H24070300003</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>πουκαμισο</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>INV000016</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:02:49</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>H24070300004</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>πουκαμισο</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>INV000017</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:04:16</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>J24070300006</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>INV000017</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2024-07-03 20:04:16</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>J24070300007</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>ζωνη</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -674,7 +1474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -701,7 +1501,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-07-03</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1299</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +1535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,7 +1562,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-07</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1299</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +1611,7 @@
         <v>2024</v>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
+        <v>1654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>